<commit_message>
stock & product detail page changes
</commit_message>
<xml_diff>
--- a/public/template/Stock.xlsx
+++ b/public/template/Stock.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9120"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,21 +27,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>product_sku</t>
+    <t>DesignNo</t>
+  </si>
+  <si>
+    <t>Jeweltype</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Subcategory</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Procatgory</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>Purity</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>style</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>making</t>
   </si>
   <si>
     <t>qty</t>
-  </si>
-  <si>
-    <t>box</t>
-  </si>
-  <si>
-    <t>purity</t>
-  </si>
-  <si>
-    <t>size</t>
   </si>
 </sst>
 </file>
@@ -54,7 +81,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="10.25"/>
       <name val="Calibri"/>
@@ -66,6 +93,13 @@
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.85"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -530,139 +564,144 @@
     <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -936,6 +975,13 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1196,33 +1242,63 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.8" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="11.5555555555556" customWidth="1"/>
-    <col min="2" max="2" width="18.1111111111111" customWidth="1"/>
+    <col min="2" max="2" width="10.2222222222222" customWidth="1"/>
+    <col min="3" max="3" width="9.44444444444444" customWidth="1"/>
+    <col min="4" max="4" width="12.8888888888889" customWidth="1"/>
+    <col min="6" max="6" width="11.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="1" customFormat="1" ht="14.4" spans="1:14">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock and style changes
</commit_message>
<xml_diff>
--- a/public/template/Stock.xlsx
+++ b/public/template/Stock.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000"/>
+    <workbookView windowWidth="28800" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,24 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>DesignNo</t>
   </si>
   <si>
     <t>Jeweltype</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Subcategory</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Procatgory</t>
   </si>
   <si>
     <t>weight</t>
@@ -1242,22 +1230,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="11.5555555555556" customWidth="1"/>
     <col min="2" max="2" width="10.2222222222222" customWidth="1"/>
-    <col min="3" max="3" width="9.44444444444444" customWidth="1"/>
-    <col min="4" max="4" width="12.8888888888889" customWidth="1"/>
-    <col min="6" max="6" width="11.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="14.4" spans="1:14">
+    <row r="1" s="1" customFormat="1" ht="14.4" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1288,18 +1273,6 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>